<commit_message>
create OT default et report
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/OT_.Default.xlsx
+++ b/lib/PHPExcel/templates/OT_.Default.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,21 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18795" windowHeight="11340" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SUBCONTRACTING" sheetId="3" r:id="rId1"/>
+    <sheet name="SSTT FR" sheetId="1" r:id="rId1"/>
+    <sheet name="SSTT EN" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="choix">'[1]Fiche de données d''essais LCF 1'!$AA$1:$AA$2</definedName>
     <definedName name="Conditions">[2]Listes!$G$3:$G$6</definedName>
     <definedName name="Statut2">[3]Listes!$B$3:$B$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">SUBCONTRACTING!$A$1:$H$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'SSTT EN'!$A$1:$I$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'SSTT FR'!$A$1:$I$28</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -36,89 +38,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Comments:</t>
-  </si>
-  <si>
-    <t>Specification</t>
-  </si>
-  <si>
-    <t>Français</t>
-  </si>
-  <si>
-    <t>Requirements</t>
-  </si>
-  <si>
-    <t>13300-B</t>
-  </si>
-  <si>
-    <t>PO#:</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2017, october 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ST</t>
-  </si>
-  <si>
-    <t>RESIDUAL STRESS</t>
-  </si>
-  <si>
-    <t>Project Information</t>
-  </si>
-  <si>
-    <t>MRSAS Job:</t>
-  </si>
-  <si>
-    <t>Final Customer references:</t>
-  </si>
-  <si>
-    <t>8043-13300</t>
-  </si>
-  <si>
-    <t>PO xxxxxxx -  Instructions xxxxxxxxxx</t>
-  </si>
-  <si>
-    <t>Material:</t>
-  </si>
-  <si>
-    <t>Drawing:</t>
-  </si>
-  <si>
-    <t>920-850-525-F</t>
-  </si>
-  <si>
-    <t>ML18PQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report Language:  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Requested Delivery Date:
-</t>
-  </si>
-  <si>
-    <t>2017, october 30</t>
-  </si>
-  <si>
-    <t>ID Specimen</t>
-  </si>
-  <si>
-    <t>- Mesure de contraintes résiduelles par DRX (destructif) suivant DMC0063 à 0 µm (3 points à 120°) et -10 µm (3 points à 120°).
-- Fourniture d'un rapport de mesure suivant le paragraphe 4.3.2 du DMC0107 
-- Retour Eprouvette chez Metcut France</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <r>
       <rPr>
         <sz val="14"/>
-        <rFont val="MS Sans Serif"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DEMANDE DE SOUS-TRAITANCE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ce document fait office de commande.</t>
+    </r>
+  </si>
+  <si>
+    <t>PO#:</t>
+  </si>
+  <si>
+    <t>A:</t>
+  </si>
+  <si>
+    <t>Contact:</t>
+  </si>
+  <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Référence METCUT:</t>
+  </si>
+  <si>
+    <t>Livraison</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Référence Client Final:</t>
+  </si>
+  <si>
+    <t>Materiau:</t>
+  </si>
+  <si>
+    <t>Format Eprouvette:</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Date de livraison demandée:</t>
+  </si>
+  <si>
+    <t>Quantité:</t>
+  </si>
+  <si>
+    <t>Specification:</t>
+  </si>
+  <si>
+    <t>Commentaires:</t>
+  </si>
+  <si>
+    <t>Référence Eprouvette</t>
+  </si>
+  <si>
+    <t>Dessin</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t>SUBCONTRACTING REQUEST</t>
@@ -126,7 +135,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="MS Sans Serif"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
@@ -136,10 +145,62 @@
       <rPr>
         <sz val="8"/>
         <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="MS Sans Serif"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t>This document acts as an open purchase order.</t>
+    </r>
+  </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>MRSAS Job:</t>
+  </si>
+  <si>
+    <t>Delivered Goods</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Final Customer Reference:</t>
+  </si>
+  <si>
+    <t>Material:</t>
+  </si>
+  <si>
+    <t>Specimen Geometry:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Requested Delivery Date:
+</t>
+  </si>
+  <si>
+    <t>Quantity:</t>
+  </si>
+  <si>
+    <t>Comments:</t>
+  </si>
+  <si>
+    <t>ID Specimen</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Date </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(YYYY-MM-DD):</t>
     </r>
   </si>
 </sst>
@@ -147,7 +208,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\,\ [$-409]mmmm\ d;@"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -160,18 +224,19 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="MS Sans Serif"/>
+      <color theme="3"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="MS Sans Serif"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="MS Sans Serif"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -182,7 +247,19 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -194,7 +271,19 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <color theme="3" tint="0.39997558519241921"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -224,6 +313,17 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -236,17 +336,6 @@
       <right style="thin">
         <color theme="4" tint="-0.499984740745262"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </left>
-      <right/>
       <top style="thin">
         <color theme="4" tint="-0.499984740745262"/>
       </top>
@@ -267,13 +356,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
       <right style="thin">
         <color theme="4" tint="-0.499984740745262"/>
       </right>
-      <top style="thin">
-        <color theme="4" tint="-0.499984740745262"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="-0.499984740745262"/>
       </bottom>
@@ -283,33 +372,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -317,20 +461,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -360,16 +495,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>215349</xdr:colOff>
+      <xdr:colOff>162962</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
+        <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B66E9D3-A1F2-4D77-95AD-EC1A1CBA43C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{376B54B1-1CF3-4563-8CA0-5872E8592DCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -392,8 +527,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="723900" y="314325"/>
-          <a:ext cx="743987" cy="766763"/>
+          <a:off x="0" y="314325"/>
+          <a:ext cx="743987" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -427,23 +562,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>238126</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457201</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{620D646B-415E-44E3-A888-EF6863592ED2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E18AD1-7A85-434C-B348-8B9DBE5388DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -465,8 +600,187 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6038851" y="0"/>
-          <a:ext cx="476250" cy="2100263"/>
+          <a:off x="6467476" y="0"/>
+          <a:ext cx="476250" cy="2238375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF990B9C-4D48-4384-BB5D-67A4AD941258}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6467476" y="0"/>
+          <a:ext cx="476250" cy="2238375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>162962</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9964A9C6-3E43-4559-9B03-03EB8D8FC535}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="314325"/>
+          <a:ext cx="743987" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A02B8A95-6ACC-4248-803A-8DBF0DBEC62E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6467476" y="0"/>
+          <a:ext cx="476250" cy="2238375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1022,219 +1336,483 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" style="1"/>
-    <col min="5" max="5" width="50.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="1.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="1.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:7" ht="60.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="2" t="s">
+    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:11" ht="60.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="3"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="12"/>
+      <c r="E5" s="18"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="10" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="F12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+    </row>
+    <row r="20" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+    </row>
+    <row r="25" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+  </mergeCells>
+  <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.35433070866141736" bottom="0.55118110236220474" header="0.11811023622047245" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;K04-044M&amp;"Arial,Normal"&amp;8ETCUT RECHERCHES S.A.S.
+22 rue du Moulin de la Garde – 44477 CARQUEFOU Cedex  (Nantes) FRANCE – Tel. +33 240 252 507 – www.metcutfrance.com
+S.A.S. au capital de 206 250€ - VAT FR10388107443 000 11</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="1.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:11" ht="60.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="3"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="10" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="F12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="D13" s="12"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+    </row>
+    <row r="20" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+    </row>
+    <row r="25" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="D19" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
-        <v>54848684</v>
-      </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" ht="24.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" ht="24.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="1:7" ht="24.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E31" s="19"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
+  <mergeCells count="13">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.55118110236220474" header="0.11811023622047245" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.35433070866141736" bottom="0.55118110236220474" header="0.11811023622047245" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter xml:space="preserve">&amp;C&amp;K04-047M&amp;"Arial,Normal"&amp;8ETCUT RECHERCHES S.A.S.
+    <oddFooter>&amp;C&amp;K04-044M&amp;"Arial,Normal"&amp;8ETCUT RECHERCHES S.A.S.
 22 rue du Moulin de la Garde – 44477 CARQUEFOU Cedex  (Nantes) FRANCE – Tel. +33 240 252 507 – www.metcutfrance.com
-S.A.S. au capital de 206 250€ - R.C.S. Nantes B 388 104 443 </oddFooter>
+S.A.S. au capital de 206 250€ - VAT FR10388107443 000 11</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
OT ST + correction bug couleur
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/OT_.Default.xlsx
+++ b/lib/PHPExcel/templates/OT_.Default.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GPM\www\GPM\lib\PHPExcel\templates\"/>
@@ -24,10 +24,10 @@
     <definedName name="choix">'[1]Fiche de données d''essais LCF 1'!$AA$1:$AA$2</definedName>
     <definedName name="Conditions">[2]Listes!$G$3:$G$6</definedName>
     <definedName name="Statut2">[3]Listes!$B$3:$B$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'SSTT EN'!$A$1:$I$30</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'SSTT FR'!$A$1:$I$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'SSTT EN'!$A$1:$I$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'SSTT FR'!$A$1:$I$29</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -203,6 +203,26 @@
       <t>(YYYY-MM-DD):</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Pricing; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ref Devis: </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Date </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(YYYY-MM-DD):</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -211,7 +231,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\,\ [$-409]mmmm\ d;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -288,8 +308,44 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +355,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8497B0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -455,17 +517,72 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,6 +590,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF203764"/>
+      <color rgb="FF8497B0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -620,8 +743,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>233362</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -650,8 +773,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6467476" y="0"/>
-          <a:ext cx="476250" cy="2238375"/>
+          <a:off x="6581776" y="0"/>
+          <a:ext cx="476250" cy="2476500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -749,8 +872,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -779,8 +902,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6467476" y="0"/>
-          <a:ext cx="476250" cy="2238375"/>
+          <a:off x="6581776" y="0"/>
+          <a:ext cx="476250" cy="2481263"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1039,7 +1162,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007-2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1047,34 +1170,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -1336,10 +1459,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:H18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1388,56 +1511,56 @@
     </row>
     <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B6" s="15"/>
       <c r="C6" s="12"/>
+      <c r="E6" s="18"/>
       <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="12"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="10" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+    <row r="8" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="11" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="F12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="K12" s="4"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="F13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="12"/>
       <c r="F14" s="8"/>
@@ -1446,7 +1569,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="12"/>
       <c r="F15" s="8"/>
@@ -1454,115 +1577,124 @@
       <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="20" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="21" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-    </row>
-    <row r="23" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-    </row>
-    <row r="25" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+    </row>
+    <row r="26" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="13" t="s">
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E26" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.35433070866141736" bottom="0.55118110236220474" header="0.11811023622047245" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1580,10 +1712,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:H18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1614,198 +1746,214 @@
       <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="55"/>
       <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="12"/>
+      <c r="A5" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="53"/>
       <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="53"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="53"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:11" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="10" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="B8" s="54"/>
+      <c r="C8" s="53"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="11" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="F12" s="5" t="s">
+      <c r="C13" s="54"/>
+      <c r="D13" s="53"/>
+      <c r="F13" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G13" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="H13" s="36"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="C14" s="54"/>
+      <c r="D14" s="53"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="C15" s="54"/>
+      <c r="D15" s="53"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="53"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="20" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="21" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    </row>
+    <row r="22" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-    </row>
-    <row r="23" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+    </row>
+    <row r="24" spans="1:11" ht="55.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-    </row>
-    <row r="25" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+    </row>
+    <row r="26" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="13" t="s">
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E26" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="42"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="E26:H26"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.35433070866141736" bottom="0.55118110236220474" header="0.11811023622047245" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>